<commit_message>
hope this doesnt break
</commit_message>
<xml_diff>
--- a/Kerntaak 1/Datadictionary.xlsx
+++ b/Kerntaak 1/Datadictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="65">
   <si>
     <t>Data</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>lkjd</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S36"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1260,9 @@
       <c r="B20" t="s">
         <v>22</v>
       </c>
+      <c r="L20" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
@@ -1406,6 +1415,11 @@
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J36" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>